<commit_message>
Agregada funcionalidad a la actividad Signo
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="6380" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="1600" yWindow="4800" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -81,10 +81,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,13 +123,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,12 +420,13 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -498,5 +527,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>